<commit_message>
ch2 uploads, not yet built
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdoughe2/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdoughe2/GitHub/book/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A51DC97-C45C-AA4F-A8AF-5E9B36429A6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E84F9B0-FA9D-AD40-9D67-007019B6D3F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16540" xr2:uid="{26D0723B-1839-8E41-841F-866FC6073B09}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>bananas</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>year</t>
+  </si>
+  <si>
+    <t>total</t>
   </si>
 </sst>
 </file>
@@ -396,15 +399,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{383015FA-2156-D24A-AB38-31143000F0E8}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -417,8 +420,11 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -431,8 +437,12 @@
       <c r="D2">
         <v>44</v>
       </c>
+      <c r="E2">
+        <f>SUM(B2:D2)</f>
+        <v>165</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -445,8 +455,12 @@
       <c r="D3">
         <v>55</v>
       </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E4" si="0">SUM(B3:D3)</f>
+        <v>110</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -458,9 +472,16 @@
       </c>
       <c r="D4">
         <v>66</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="E2:E4" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>